<commit_message>
sprint 4 - parth
</commit_message>
<xml_diff>
--- a/Sprint4/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Sprint4/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vedadnya_98/Documents/GitHub/CS-555-Agile_Project_Team/Sprint3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Documents/Spring2020/CS555/Project04/CS-555-Agile_Project_Team/Sprint4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616B20B6-16AF-434D-BA3C-48939A980863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AA9D84-A604-F643-BFF7-8DCBE2E01DD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="324">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1018,6 +1016,36 @@
   </si>
   <si>
     <t>28-34</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>US31()</t>
+  </si>
+  <si>
+    <t>US32()</t>
+  </si>
+  <si>
+    <t>test_userstory31()</t>
+  </si>
+  <si>
+    <t>test_userstory32()</t>
+  </si>
+  <si>
+    <t>971-993</t>
+  </si>
+  <si>
+    <t>999-1019</t>
+  </si>
+  <si>
+    <t>135-138</t>
+  </si>
+  <si>
+    <t>140-144</t>
+  </si>
+  <si>
+    <t>commit without discussing</t>
   </si>
 </sst>
 </file>
@@ -1644,6 +1672,9 @@
                 <c:pt idx="3">
                   <c:v>42458</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42478</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1664,6 +1695,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3294,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:D34"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3901,7 +3935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="150" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -4096,7 +4130,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4223,6 +4257,18 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>278</v>
+      </c>
+      <c r="B6" s="13">
+        <v>42478</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="F6" s="35">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -5210,8 +5256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C20" sqref="B16:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5699,16 +5745,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14" x14ac:dyDescent="0.15">
@@ -5769,10 +5818,40 @@
         <v>182</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
       <c r="E2">
         <v>50</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K2" t="s">
+        <v>315</v>
+      </c>
+      <c r="L2" t="s">
+        <v>319</v>
+      </c>
+      <c r="M2" t="s">
+        <v>212</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
@@ -5785,11 +5864,41 @@
       <c r="C3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D3" t="s">
-        <v>292</v>
+      <c r="D3" s="32" t="s">
+        <v>314</v>
       </c>
       <c r="E3">
         <v>50</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K3" t="s">
+        <v>316</v>
+      </c>
+      <c r="L3" t="s">
+        <v>320</v>
+      </c>
+      <c r="M3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -5808,6 +5917,12 @@
       <c r="E4">
         <v>50</v>
       </c>
+      <c r="J4" t="s">
+        <v>241</v>
+      </c>
+      <c r="M4" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
@@ -5825,6 +5940,12 @@
       <c r="E5">
         <v>50</v>
       </c>
+      <c r="J5" t="s">
+        <v>241</v>
+      </c>
+      <c r="M5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
@@ -5842,6 +5963,12 @@
       <c r="E6">
         <v>50</v>
       </c>
+      <c r="J6" t="s">
+        <v>241</v>
+      </c>
+      <c r="M6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="21" t="s">
@@ -5859,6 +5986,12 @@
       <c r="E7">
         <v>50</v>
       </c>
+      <c r="J7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M7" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="30" t="s">
@@ -5876,6 +6009,12 @@
       <c r="E8">
         <v>50</v>
       </c>
+      <c r="J8" t="s">
+        <v>241</v>
+      </c>
+      <c r="M8" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="30" t="s">
@@ -5893,8 +6032,59 @@
       <c r="E9">
         <v>50</v>
       </c>
+      <c r="J9" t="s">
+        <v>241</v>
+      </c>
+      <c r="M9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C19:G19"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5904,8 +6094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:B40"/>
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>